<commit_message>
shape file editing for Earth Engine
</commit_message>
<xml_diff>
--- a/maxs_work/bulletin_132_work/transfers_by_seller_new.xlsx
+++ b/maxs_work/bulletin_132_work/transfers_by_seller_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxslesinski/Documents/GitHub/dlkency_CALFEWS/CALFEWS/maxs_work/bulletin_132_work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS/maxs_work/bulletin_132_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778250DA-C4C7-0745-9100-819F180E1D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{778250DA-C4C7-0745-9100-819F180E1D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D88932D-3E71-4A63-A9F0-7E266B35135F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15040" windowHeight="16280" xr2:uid="{CAEF76C3-CC13-994B-AF76-6F3F7E947AA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CAEF76C3-CC13-994B-AF76-6F3F7E947AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,15 +522,17 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -553,7 +555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -570,7 +572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -587,7 +589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -604,7 +606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -621,7 +623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -638,7 +640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -655,7 +657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -672,7 +674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -689,7 +691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -706,7 +708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -723,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -740,7 +742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -757,7 +759,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -774,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -791,7 +793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -808,7 +810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -825,7 +827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -842,7 +844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -859,7 +861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -876,7 +878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -893,7 +895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -910,7 +912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -927,7 +929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -944,7 +946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -961,7 +963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -978,7 +980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -995,7 +997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1029,7 +1031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1080,7 +1082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1097,7 +1099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1131,7 +1133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1148,7 +1150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -1182,7 +1184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>13</v>
       </c>

</xml_diff>